<commit_message>
added materials onboarding updated opacity
</commit_message>
<xml_diff>
--- a/data/materials_generator/suppliers.xlsx
+++ b/data/materials_generator/suppliers.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1273" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1275" uniqueCount="475">
   <si>
     <t>TOP3D</t>
   </si>
@@ -9149,9 +9149,6 @@
     <t>Russia</t>
   </si>
   <si>
-    <t>NinjaTek, www.ninjatek.com NinjaFlex</t>
-  </si>
-  <si>
     <t>Monoprice.Com 3d printer Filament</t>
   </si>
   <si>
@@ -9165,6 +9162,12 @@
   </si>
   <si>
     <t>need to add NGEN product line</t>
+  </si>
+  <si>
+    <t>review to make sure prices okay and didn't miss items</t>
+  </si>
+  <si>
+    <t>NinjaTek, http://www.ninjaflex3d.com/, NinjaFlex</t>
   </si>
 </sst>
 </file>
@@ -9392,20 +9395,20 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -11350,8 +11353,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H255"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="L83" sqref="L83"/>
+    <sheetView tabSelected="1" topLeftCell="A248" workbookViewId="0">
+      <selection activeCell="H249" sqref="H249"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11381,11 +11384,11 @@
       <c r="F1" s="14" t="s">
         <v>384</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="G1" s="25" t="s">
+        <v>470</v>
+      </c>
+      <c r="H1" s="25" t="s">
         <v>471</v>
-      </c>
-      <c r="H1" s="28" t="s">
-        <v>472</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -11621,8 +11624,8 @@
         <v>3</v>
       </c>
       <c r="F14" s="7"/>
-      <c r="G14" s="29" t="s">
-        <v>470</v>
+      <c r="G14" s="26" t="s">
+        <v>469</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="26.25">
@@ -12470,11 +12473,11 @@
       <c r="F61" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G61" s="30" t="s">
-        <v>470</v>
-      </c>
-      <c r="H61" s="30" t="s">
-        <v>473</v>
+      <c r="G61" s="27" t="s">
+        <v>469</v>
+      </c>
+      <c r="H61" s="27" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -12492,7 +12495,7 @@
       </c>
       <c r="E62" s="7"/>
       <c r="F62" s="7"/>
-      <c r="G62" s="29"/>
+      <c r="G62" s="26"/>
     </row>
     <row r="63" spans="1:8">
       <c r="A63" s="15" t="s">
@@ -12696,7 +12699,7 @@
       <c r="E74" s="12"/>
       <c r="F74" s="12"/>
       <c r="G74" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="30">
@@ -13387,7 +13390,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="113" spans="1:6">
+    <row r="113" spans="1:8">
       <c r="A113" s="17" t="s">
         <v>198</v>
       </c>
@@ -13405,7 +13408,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="114" spans="1:6">
+    <row r="114" spans="1:8">
       <c r="A114" s="6" t="s">
         <v>199</v>
       </c>
@@ -13423,7 +13426,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="115" spans="1:6">
+    <row r="115" spans="1:8">
       <c r="A115" s="6" t="s">
         <v>200</v>
       </c>
@@ -13441,7 +13444,7 @@
       </c>
       <c r="F115" s="7"/>
     </row>
-    <row r="116" spans="1:6">
+    <row r="116" spans="1:8">
       <c r="A116" s="6" t="s">
         <v>201</v>
       </c>
@@ -13459,7 +13462,7 @@
       </c>
       <c r="F116" s="7"/>
     </row>
-    <row r="117" spans="1:6" ht="39">
+    <row r="117" spans="1:8" ht="39">
       <c r="A117" s="17" t="s">
         <v>203</v>
       </c>
@@ -13477,7 +13480,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="118" spans="1:6">
+    <row r="118" spans="1:8">
       <c r="A118" s="6" t="s">
         <v>206</v>
       </c>
@@ -13495,7 +13498,7 @@
       </c>
       <c r="F118" s="7"/>
     </row>
-    <row r="119" spans="1:6" ht="39">
+    <row r="119" spans="1:8" ht="39">
       <c r="A119" s="6" t="s">
         <v>209</v>
       </c>
@@ -13515,7 +13518,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="120" spans="1:6">
+    <row r="120" spans="1:8" ht="102.75">
       <c r="A120" s="17" t="s">
         <v>211</v>
       </c>
@@ -13532,8 +13535,14 @@
         <v>3</v>
       </c>
       <c r="F120" s="7"/>
-    </row>
-    <row r="121" spans="1:6">
+      <c r="G120" s="26" t="s">
+        <v>469</v>
+      </c>
+      <c r="H120" s="26" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8">
       <c r="A121" s="16" t="s">
         <v>212</v>
       </c>
@@ -13553,7 +13562,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="122" spans="1:6">
+    <row r="122" spans="1:8">
       <c r="A122" s="16" t="s">
         <v>213</v>
       </c>
@@ -13571,7 +13580,7 @@
       </c>
       <c r="F122" s="7"/>
     </row>
-    <row r="123" spans="1:6" ht="26.25">
+    <row r="123" spans="1:8" ht="26.25">
       <c r="A123" s="17" t="s">
         <v>214</v>
       </c>
@@ -13589,7 +13598,7 @@
       </c>
       <c r="F123" s="7"/>
     </row>
-    <row r="124" spans="1:6">
+    <row r="124" spans="1:8">
       <c r="A124" s="16" t="s">
         <v>216</v>
       </c>
@@ -13609,7 +13618,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="125" spans="1:6" ht="26.25">
+    <row r="125" spans="1:8" ht="26.25">
       <c r="A125" s="17" t="s">
         <v>217</v>
       </c>
@@ -13627,7 +13636,7 @@
       </c>
       <c r="F125" s="7"/>
     </row>
-    <row r="126" spans="1:6">
+    <row r="126" spans="1:8">
       <c r="A126" s="6" t="s">
         <v>218</v>
       </c>
@@ -13647,7 +13656,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="127" spans="1:6">
+    <row r="127" spans="1:8">
       <c r="A127" s="17" t="s">
         <v>219</v>
       </c>
@@ -13663,7 +13672,7 @@
       <c r="E127" s="7"/>
       <c r="F127" s="7"/>
     </row>
-    <row r="128" spans="1:6" ht="39">
+    <row r="128" spans="1:8" ht="39">
       <c r="A128" s="17" t="s">
         <v>221</v>
       </c>
@@ -13705,39 +13714,39 @@
       <c r="A130" s="16" t="s">
         <v>224</v>
       </c>
-      <c r="B130" s="25" t="s">
+      <c r="B130" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C130" s="27" t="s">
+      <c r="C130" s="29" t="s">
         <v>227</v>
       </c>
-      <c r="D130" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="E130" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="F130" s="25"/>
+      <c r="D130" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="E130" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="F130" s="28"/>
     </row>
     <row r="131" spans="1:6">
       <c r="A131" s="16" t="s">
         <v>225</v>
       </c>
-      <c r="B131" s="25"/>
-      <c r="C131" s="27"/>
-      <c r="D131" s="25"/>
-      <c r="E131" s="25"/>
-      <c r="F131" s="25"/>
+      <c r="B131" s="28"/>
+      <c r="C131" s="29"/>
+      <c r="D131" s="28"/>
+      <c r="E131" s="28"/>
+      <c r="F131" s="28"/>
     </row>
     <row r="132" spans="1:6">
       <c r="A132" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="B132" s="25"/>
-      <c r="C132" s="27"/>
-      <c r="D132" s="25"/>
-      <c r="E132" s="25"/>
-      <c r="F132" s="25"/>
+      <c r="B132" s="28"/>
+      <c r="C132" s="29"/>
+      <c r="D132" s="28"/>
+      <c r="E132" s="28"/>
+      <c r="F132" s="28"/>
     </row>
     <row r="133" spans="1:6" ht="26.25">
       <c r="A133" s="6" t="s">
@@ -15210,19 +15219,19 @@
       <c r="F214" s="7"/>
     </row>
     <row r="215" spans="1:6">
-      <c r="A215" s="25" t="s">
+      <c r="A215" s="28" t="s">
         <v>346</v>
       </c>
-      <c r="B215" s="25" t="s">
+      <c r="B215" s="28" t="s">
         <v>347</v>
       </c>
-      <c r="C215" s="26" t="s">
+      <c r="C215" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="D215" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="E215" s="25" t="s">
+      <c r="D215" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="E215" s="28" t="s">
         <v>3</v>
       </c>
       <c r="F215" s="7" t="s">
@@ -15230,21 +15239,21 @@
       </c>
     </row>
     <row r="216" spans="1:6" ht="409.6">
-      <c r="A216" s="25"/>
-      <c r="B216" s="25"/>
-      <c r="C216" s="26"/>
-      <c r="D216" s="25"/>
-      <c r="E216" s="25"/>
+      <c r="A216" s="28"/>
+      <c r="B216" s="28"/>
+      <c r="C216" s="30"/>
+      <c r="D216" s="28"/>
+      <c r="E216" s="28"/>
       <c r="F216" s="7" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="217" spans="1:6" ht="409.6">
-      <c r="A217" s="25"/>
-      <c r="B217" s="25"/>
-      <c r="C217" s="26"/>
-      <c r="D217" s="25"/>
-      <c r="E217" s="25"/>
+      <c r="A217" s="28"/>
+      <c r="B217" s="28"/>
+      <c r="C217" s="30"/>
+      <c r="D217" s="28"/>
+      <c r="E217" s="28"/>
       <c r="F217" s="7" t="s">
         <v>350</v>
       </c>
@@ -15843,7 +15852,7 @@
     </row>
     <row r="248" spans="1:7" ht="78" thickBot="1">
       <c r="A248" s="21" t="s">
-        <v>468</v>
+        <v>474</v>
       </c>
       <c r="B248" s="2" t="s">
         <v>442</v>
@@ -15967,21 +15976,21 @@
     </row>
     <row r="255" spans="1:7">
       <c r="A255" s="24" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A215:A217"/>
+    <mergeCell ref="B215:B217"/>
+    <mergeCell ref="C215:C217"/>
+    <mergeCell ref="D215:D217"/>
+    <mergeCell ref="E215:E217"/>
     <mergeCell ref="B130:B132"/>
     <mergeCell ref="C130:C132"/>
     <mergeCell ref="D130:D132"/>
     <mergeCell ref="E130:E132"/>
     <mergeCell ref="F130:F132"/>
-    <mergeCell ref="A215:A217"/>
-    <mergeCell ref="B215:B217"/>
-    <mergeCell ref="C215:C217"/>
-    <mergeCell ref="D215:D217"/>
-    <mergeCell ref="E215:E217"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="http://en.top3d.co.kr/"/>

</xml_diff>